<commit_message>
fix: mengandung boolean, pindah reten promosi ke regular, kepp reten tambah formula kt excel, tambah version kononnya
</commit_message>
<xml_diff>
--- a/public/exports/KEPP.xlsx
+++ b/public/exports/KEPP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vault\Project\giret extreme\baru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calypso\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AD9AAD-F821-441C-8333-7D46D5DD834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA76255-E676-4809-822F-C5DDCA0D7A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KEPP" sheetId="1" r:id="rId1"/>
@@ -522,19 +522,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -545,8 +536,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -770,7 +770,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -836,7 +836,7 @@
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="25"/>
       <c r="D4" s="26"/>
       <c r="K4" s="9" t="s">
@@ -850,7 +850,7 @@
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="25"/>
       <c r="D5" s="26"/>
       <c r="T5" s="10" t="s">
@@ -861,7 +861,7 @@
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="35"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="25"/>
       <c r="D6" s="26"/>
       <c r="T6" s="10" t="s">
@@ -873,17 +873,17 @@
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:20" ht="25.5" customHeight="1">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="26"/>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="35" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="25"/>
@@ -907,39 +907,39 @@
       <c r="T8" s="26"/>
     </row>
     <row r="9" spans="1:20" ht="58.5" customHeight="1">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="27" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="K9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="33" t="s">
         <v>24</v>
       </c>
       <c r="N9" s="24" t="s">
@@ -947,16 +947,16 @@
       </c>
       <c r="O9" s="25"/>
       <c r="P9" s="26"/>
-      <c r="Q9" s="27" t="s">
+      <c r="Q9" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="R9" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="S9" s="27" t="s">
+      <c r="S9" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="T9" s="27" t="s">
+      <c r="T9" s="33" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14">
-        <f>SUM(C12:H12)</f>
+        <f>SUM(E12:H12)</f>
         <v>0</v>
       </c>
       <c r="J12" s="13"/>
@@ -1088,7 +1088,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14">
-        <f t="shared" ref="I13:I24" si="0">SUM(C13:H13)</f>
+        <f t="shared" ref="I13:I24" si="0">SUM(E13:H13)</f>
         <v>0</v>
       </c>
       <c r="J13" s="13"/>
@@ -1426,17 +1426,17 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:20" ht="92.25" customHeight="1">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
     </row>
     <row r="27" spans="1:20" ht="24.75" customHeight="1">
       <c r="A27" s="16"/>
@@ -2469,17 +2469,6 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="J8:Q8"/>
     <mergeCell ref="R8:T8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -2495,6 +2484,17 @@
     <mergeCell ref="K9:K10"/>
     <mergeCell ref="L9:L10"/>
     <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="J8:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>

</xml_diff>